<commit_message>
journal de travail à jour et ajout de l'annexe
</commit_message>
<xml_diff>
--- a/133_GESTPROJ_G02.xlsx
+++ b/133_GESTPROJ_G02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\133 - HAY\EMF-Shelf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3ème année\Module 133\EMF-Shelf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490382FA-FAB4-42A1-A1DF-B06A73B9D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AA4899-EE31-4E33-AF9B-EDCEC1ACA552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Planning</t>
   </si>
@@ -322,12 +321,27 @@
   <si>
     <t>REST des comptes</t>
   </si>
+  <si>
+    <t>Exercice 10</t>
+  </si>
+  <si>
+    <t>REST des livres</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,20 +425,6 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="6"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -827,7 +827,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -840,21 +840,12 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,21 +885,9 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -946,6 +925,93 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1291,8 +1357,8 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1302,67 +1368,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="35"/>
       <c r="O3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="54">
+      <c r="P3" s="33">
         <v>300233</v>
       </c>
-      <c r="Q3" s="56"/>
+      <c r="Q3" s="35"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="56"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="35"/>
       <c r="O4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1372,467 +1438,493 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="57" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="57" t="s">
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="57" t="s">
+      <c r="I7" s="37"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="57" t="s">
+      <c r="M7" s="37"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="59"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="8" t="s">
+      <c r="K8" s="10"/>
+      <c r="L8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="50" t="s">
+      <c r="B9" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="43"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="13"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="49"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="13"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="49"/>
     </row>
     <row r="11" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="13"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="50"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="49"/>
     </row>
     <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="13"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="43"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="49"/>
     </row>
     <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="13"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="49"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="13"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="49"/>
     </row>
     <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="13"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="49"/>
     </row>
     <row r="16" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="13"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="49"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="13"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="49"/>
     </row>
     <row r="18" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="13"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="53"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
     </row>
     <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="13"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="44"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="49"/>
     </row>
     <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="13"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="44"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="49"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="13"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="49"/>
     </row>
     <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="13"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="49"/>
     </row>
     <row r="23" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="13"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="49"/>
     </row>
     <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="34"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="58"/>
     </row>
     <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="39"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="67"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="45"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1865,8 +1957,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,18 +1969,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="2"/>
@@ -1897,147 +1989,147 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="16">
         <v>45016</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="17">
         <v>1.75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="16">
         <v>45016</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="17">
         <v>1.75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="16">
         <v>45016</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="17">
         <v>3.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="26"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="26">
+      <c r="B22" s="13"/>
+      <c r="C22" s="17">
         <f>SUM(C8:C21)</f>
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="20" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2062,7 +2154,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,18 +2165,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="15" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="2"/>
@@ -2093,131 +2185,147 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="16">
         <v>45016</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="17">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="26"/>
+      <c r="A9" s="16">
+        <v>45016</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="16">
+        <v>45016</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="17">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="26"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="26">
+      <c r="B22" s="13"/>
+      <c r="C22" s="17">
         <f>SUM(C8:C21)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="20" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2235,59 +2343,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2733,21 +2794,65 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2773,9 +2878,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
+    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>